<commit_message>
subtlee changes on what hafiz made
</commit_message>
<xml_diff>
--- a/INVENTARIOS DEPOSITO/BAJADA A TIENDA 05-08.xlsx
+++ b/INVENTARIOS DEPOSITO/BAJADA A TIENDA 05-08.xlsx
@@ -597,16 +597,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z69"/>
+  <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA68" activeCellId="0" sqref="AA68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.28"/>
@@ -2584,7 +2584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>81</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>82</v>
       </c>
@@ -2689,6 +2689,9 @@
       <c r="V35" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W35" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X35" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>85</v>
       </c>
@@ -2745,6 +2748,9 @@
       <c r="V36" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W36" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X36" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -2755,7 +2761,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>86</v>
       </c>
@@ -2801,6 +2807,9 @@
       <c r="V37" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W37" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X37" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>87</v>
       </c>
@@ -2857,6 +2866,9 @@
       <c r="V38" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W38" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X38" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -2867,7 +2879,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>88</v>
       </c>
@@ -2913,6 +2925,9 @@
       <c r="V39" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W39" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X39" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -2923,7 +2938,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>89</v>
       </c>
@@ -2969,6 +2984,9 @@
       <c r="V40" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W40" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X40" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -2979,7 +2997,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>90</v>
       </c>
@@ -3025,6 +3043,9 @@
       <c r="V41" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W41" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X41" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3035,7 +3056,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>91</v>
       </c>
@@ -3081,6 +3102,9 @@
       <c r="V42" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W42" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X42" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3091,7 +3115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>92</v>
       </c>
@@ -3137,6 +3161,9 @@
       <c r="V43" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W43" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X43" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3147,7 +3174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>93</v>
       </c>
@@ -3193,6 +3220,9 @@
       <c r="V44" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W44" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X44" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3203,7 +3233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>94</v>
       </c>
@@ -3249,6 +3279,9 @@
       <c r="V45" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W45" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X45" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3259,7 +3292,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>97</v>
       </c>
@@ -3305,6 +3338,9 @@
       <c r="V46" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W46" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X46" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3315,7 +3351,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>98</v>
       </c>
@@ -3361,6 +3397,9 @@
       <c r="V47" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W47" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X47" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3371,7 +3410,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>99</v>
       </c>
@@ -3417,6 +3456,9 @@
       <c r="V48" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W48" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X48" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3427,7 +3469,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>100</v>
       </c>
@@ -3473,6 +3515,9 @@
       <c r="V49" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W49" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X49" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3483,7 +3528,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>101</v>
       </c>
@@ -3529,6 +3574,9 @@
       <c r="V50" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W50" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X50" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3539,7 +3587,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>104</v>
       </c>
@@ -3585,6 +3633,9 @@
       <c r="V51" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W51" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X51" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3595,7 +3646,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>105</v>
       </c>
@@ -3641,6 +3692,9 @@
       <c r="V52" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W52" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X52" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3651,7 +3705,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>106</v>
       </c>
@@ -3697,6 +3751,9 @@
       <c r="V53" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W53" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X53" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3707,7 +3764,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>107</v>
       </c>
@@ -3753,6 +3810,9 @@
       <c r="V54" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W54" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X54" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3763,7 +3823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>108</v>
       </c>
@@ -3809,6 +3869,9 @@
       <c r="V55" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W55" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X55" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3819,7 +3882,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>109</v>
       </c>
@@ -3865,6 +3928,9 @@
       <c r="V56" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W56" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X56" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3875,7 +3941,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>110</v>
       </c>
@@ -3921,6 +3987,9 @@
       <c r="V57" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W57" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X57" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3931,7 +4000,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>111</v>
       </c>
@@ -3977,6 +4046,9 @@
       <c r="V58" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W58" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X58" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -3987,7 +4059,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>112</v>
       </c>
@@ -4033,6 +4105,9 @@
       <c r="V59" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W59" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X59" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4043,7 +4118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>113</v>
       </c>
@@ -4089,6 +4164,9 @@
       <c r="V60" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W60" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X60" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4099,7 +4177,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>116</v>
       </c>
@@ -4145,6 +4223,9 @@
       <c r="V61" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W61" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X61" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4155,7 +4236,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>117</v>
       </c>
@@ -4201,6 +4282,9 @@
       <c r="V62" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W62" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X62" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4211,7 +4295,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>118</v>
       </c>
@@ -4257,6 +4341,9 @@
       <c r="V63" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W63" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X63" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4267,7 +4354,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>119</v>
       </c>
@@ -4313,6 +4400,9 @@
       <c r="V64" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W64" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X64" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4323,7 +4413,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>120</v>
       </c>
@@ -4369,6 +4459,9 @@
       <c r="V65" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W65" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X65" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4379,7 +4472,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>121</v>
       </c>
@@ -4425,6 +4518,9 @@
       <c r="V66" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W66" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X66" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4435,7 +4531,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>122</v>
       </c>
@@ -4481,6 +4577,9 @@
       <c r="V67" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W67" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X67" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4491,7 +4590,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>123</v>
       </c>
@@ -4537,6 +4636,9 @@
       <c r="V68" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W68" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X68" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4547,7 +4649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>124</v>
       </c>
@@ -4593,6 +4695,9 @@
       <c r="V69" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W69" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="X69" s="0" t="n">
         <v>25998807</v>
       </c>
@@ -4603,6 +4708,13 @@
         <v>115</v>
       </c>
     </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>